<commit_message>
added lab 01 assignment
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F3D170-34DD-A14A-9B93-9988E57F4037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CA2405-CF76-8944-9F5B-F85245BF67A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Assignment</t>
   </si>
@@ -101,9 +101,6 @@
     <t>December 04, 2024</t>
   </si>
   <si>
-    <t>lab1</t>
-  </si>
-  <si>
     <t>September 11, 2024</t>
   </si>
   <si>
@@ -111,6 +108,12 @@
   </si>
   <si>
     <t>September 25, 2024</t>
+  </si>
+  <si>
+    <t>SA1</t>
+  </si>
+  <si>
+    <t>September 09, 2024</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -501,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -509,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -578,7 +581,10 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date for short assignment 2
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CA2405-CF76-8944-9F5B-F85245BF67A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA9095-C9EF-1442-B52A-1E1B4AED1D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Assignment</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>September 09, 2024</t>
+  </si>
+  <si>
+    <t>September 16, 2024</t>
+  </si>
+  <si>
+    <t>SA2</t>
   </si>
 </sst>
 </file>
@@ -472,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,6 +593,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added short assignment 3 deadline
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA9095-C9EF-1442-B52A-1E1B4AED1D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D44B7-6DB5-004D-922A-8776B0CF51FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Assignment</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>SA2</t>
+  </si>
+  <si>
+    <t>SA3</t>
+  </si>
+  <si>
+    <t>September 23, 2024</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,6 +607,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added lab 04 instructions and images
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D44B7-6DB5-004D-922A-8776B0CF51FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F951D527-E1F5-D54C-9520-9B21EE33BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Assignment</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>September 23, 2024</t>
+  </si>
+  <si>
+    <t>SA4</t>
+  </si>
+  <si>
+    <t>September 30, 2024</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,6 +621,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added pa4 instructions and links
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F951D527-E1F5-D54C-9520-9B21EE33BBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B55F483-9497-7E42-93C3-F15DA3B4DB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>PA11</t>
   </si>
   <si>
-    <t>October 02, 2024</t>
-  </si>
-  <si>
     <t>October 09, 2024</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>September 18, 2024</t>
   </si>
   <si>
-    <t>September 25, 2024</t>
-  </si>
-  <si>
     <t>SA1</t>
   </si>
   <si>
@@ -132,6 +126,12 @@
   </si>
   <si>
     <t>September 30, 2024</t>
+  </si>
+  <si>
+    <t>September 27, 2024</t>
+  </si>
+  <si>
+    <t>October 04, 2024</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -522,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -530,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -538,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -554,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -578,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -594,39 +594,39 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added lab 5 link
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B55F483-9497-7E42-93C3-F15DA3B4DB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0597EA2-BC2B-1044-B705-872D832C1935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Assignment</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>October 04, 2024</t>
+  </si>
+  <si>
+    <t>SA5</t>
+  </si>
+  <si>
+    <t>October 06, 2024</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,6 +635,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added instructions and links for pa5
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0597EA2-BC2B-1044-B705-872D832C1935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A946583-C9A7-FE47-BA65-06EBA8FF908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>PA4</t>
   </si>
   <si>
-    <t>PA5</t>
-  </si>
-  <si>
     <t>PA6</t>
   </si>
   <si>
@@ -74,21 +71,12 @@
     <t>PA10</t>
   </si>
   <si>
-    <t>PA11</t>
-  </si>
-  <si>
-    <t>October 09, 2024</t>
-  </si>
-  <si>
     <t>October 30, 2024</t>
   </si>
   <si>
     <t>October 23, 2024</t>
   </si>
   <si>
-    <t>November 13, 2024</t>
-  </si>
-  <si>
     <t>November 20, 2024</t>
   </si>
   <si>
@@ -138,6 +126,18 @@
   </si>
   <si>
     <t>October 06, 2024</t>
+  </si>
+  <si>
+    <t>October 11, 2024</t>
+  </si>
+  <si>
+    <t>PA5a</t>
+  </si>
+  <si>
+    <t>PA5b</t>
+  </si>
+  <si>
+    <t>October 16, 2024</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -528,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -536,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -544,103 +544,103 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated deadline for SA5
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A946583-C9A7-FE47-BA65-06EBA8FF908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072FDBB8-D449-A347-9526-7168FB03AAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>SA5</t>
   </si>
   <si>
-    <t>October 06, 2024</t>
-  </si>
-  <si>
     <t>October 11, 2024</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>October 16, 2024</t>
+  </si>
+  <si>
+    <t>October 07, 2024</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,18 +549,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added instructions to submit UML diagram to gradescope
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072FDBB8-D449-A347-9526-7168FB03AAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87415284-1BA6-1C4E-81B4-254781C4E2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
+    <workbookView xWindow="-34660" yWindow="1140" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Assignment</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>October 07, 2024</t>
+  </si>
+  <si>
+    <t>SA6</t>
+  </si>
+  <si>
+    <t>October 09, 2024</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,6 +649,14 @@
         <v>33</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added programming assignment 6 instructions
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D879DE8D-4875-5D43-BB34-E7B9C4DC328F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DA8EA3-8ED7-8549-81A2-4B792AD08923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34660" yWindow="1140" windowWidth="28040" windowHeight="17440" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,15 +68,9 @@
     <t>PA9</t>
   </si>
   <si>
-    <t>PA10</t>
-  </si>
-  <si>
     <t>October 30, 2024</t>
   </si>
   <si>
-    <t>October 23, 2024</t>
-  </si>
-  <si>
     <t>November 20, 2024</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>October 21, 2024</t>
+  </si>
+  <si>
+    <t>SA8</t>
+  </si>
+  <si>
+    <t>October 28, 2024</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,23 +556,23 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +580,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -604,31 +604,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -641,15 +641,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
updated assignment 7 instructions
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DA8EA3-8ED7-8549-81A2-4B792AD08923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F32194-DCF7-F948-B19E-CE5462925B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>October 30, 2024</t>
   </si>
   <si>
-    <t>November 20, 2024</t>
-  </si>
-  <si>
     <t>December 11, 2024</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>October 28, 2024</t>
+  </si>
+  <si>
+    <t>November 13, 2024</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,23 +556,23 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -604,71 +604,71 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added second set of slides to module 8
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F32194-DCF7-F948-B19E-CE5462925B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E0F64-7B16-2D4B-916A-7B789D4879DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Assignment</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>November 13, 2024</t>
+  </si>
+  <si>
+    <t>SA9</t>
+  </si>
+  <si>
+    <t>November 12, 2024</t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,6 +677,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
shifted topics, added link to short assignment 10
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27E0F64-7B16-2D4B-916A-7B789D4879DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5241BD8A-7017-2345-8452-75BE43500E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Assignment</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>November 12, 2024</t>
+  </si>
+  <si>
+    <t>SA10</t>
+  </si>
+  <si>
+    <t>November 18, 2024</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,6 +691,14 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added PA9 and PA10 instructions (minimal instructions)
</commit_message>
<xml_diff>
--- a/assessment-deadlines.xlsx
+++ b/assessment-deadlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29CC7FB-88EF-EC49-86DD-64940720006F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F896A34-2193-7442-A536-517EE79FD647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{42CF13FC-3BCA-794F-8273-F6C21051D52A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Assignment</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>November 22 2024</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>December 11, 2024</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED722F87-98A2-CF4A-8920-C90E90C5E394}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,81 +627,89 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>